<commit_message>
updated artist list with SM website info
</commit_message>
<xml_diff>
--- a/data/artist_list.xlsx
+++ b/data/artist_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylergleeson/Documents/GitHub/kpop_analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59257813-3F77-6942-BA3B-A140BC5124C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8797B3DA-5FE3-434C-9402-06A8ED4E1368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
   <si>
     <t>EXO</t>
   </si>
@@ -254,9 +254,6 @@
     <t>SF9</t>
   </si>
   <si>
-    <t>ONEUS </t>
-  </si>
-  <si>
     <t>EVERGLOW</t>
   </si>
   <si>
@@ -267,6 +264,324 @@
   </si>
   <si>
     <t>MOMOLAND</t>
+  </si>
+  <si>
+    <t>ZHOUMI</t>
+  </si>
+  <si>
+    <t>YUTA</t>
+  </si>
+  <si>
+    <t>YUSHI</t>
+  </si>
+  <si>
+    <t>YURI</t>
+  </si>
+  <si>
+    <t>YOU HOJEONG</t>
+  </si>
+  <si>
+    <t>YOONA</t>
+  </si>
+  <si>
+    <t>YOON DAHOON</t>
+  </si>
+  <si>
+    <t>YESUNG</t>
+  </si>
+  <si>
+    <t>YERI</t>
+  </si>
+  <si>
+    <t>YANGYANG</t>
+  </si>
+  <si>
+    <t>XIUMIN</t>
+  </si>
+  <si>
+    <t>XIAOJUN</t>
+  </si>
+  <si>
+    <t>WONBIN</t>
+  </si>
+  <si>
+    <t>WINWIN</t>
+  </si>
+  <si>
+    <t>WINTER</t>
+  </si>
+  <si>
+    <t>WENDY</t>
+  </si>
+  <si>
+    <t>WayV-TEN&amp;YANGYANG</t>
+  </si>
+  <si>
+    <t>WayV-KUN&amp;XIAOJUN</t>
+  </si>
+  <si>
+    <t>WayV</t>
+  </si>
+  <si>
+    <t>U-Know</t>
+  </si>
+  <si>
+    <t>TVXQ!</t>
+  </si>
+  <si>
+    <t>TEN</t>
+  </si>
+  <si>
+    <t>TAEYONG</t>
+  </si>
+  <si>
+    <t>TAEYEON</t>
+  </si>
+  <si>
+    <t>TAEMIN</t>
+  </si>
+  <si>
+    <t>TAEIL</t>
+  </si>
+  <si>
+    <t>SuperM</t>
+  </si>
+  <si>
+    <t>SUPER JUNIOR-L.S.S.</t>
+  </si>
+  <si>
+    <t>SUPER JUNIOR-K.R.Y.</t>
+  </si>
+  <si>
+    <t>SUPER JUNIOR-D&amp;E</t>
+  </si>
+  <si>
+    <t>SUNGMIN</t>
+  </si>
+  <si>
+    <t>SUNGCHAN</t>
+  </si>
+  <si>
+    <t>SULLI</t>
+  </si>
+  <si>
+    <t>SUHO</t>
+  </si>
+  <si>
+    <t>SOHEE</t>
+  </si>
+  <si>
+    <t>SM The Ballad</t>
+  </si>
+  <si>
+    <t>SIWON</t>
+  </si>
+  <si>
+    <t>SION</t>
+  </si>
+  <si>
+    <t>SHOTARO</t>
+  </si>
+  <si>
+    <t>SHINDONG</t>
+  </si>
+  <si>
+    <t>SEUNGHAN</t>
+  </si>
+  <si>
+    <t>SEULGI</t>
+  </si>
+  <si>
+    <t>SEHUN</t>
+  </si>
+  <si>
+    <t>SAKUYA</t>
+  </si>
+  <si>
+    <t>RYO</t>
+  </si>
+  <si>
+    <t>RYEOWOOK</t>
+  </si>
+  <si>
+    <t>RIKU</t>
+  </si>
+  <si>
+    <t>RENJUN</t>
+  </si>
+  <si>
+    <t>Red Velvet – IRENE &amp; SEULGI</t>
+  </si>
+  <si>
+    <t>Raiden</t>
+  </si>
+  <si>
+    <t>ONEW</t>
+  </si>
+  <si>
+    <t>NINGNING</t>
+  </si>
+  <si>
+    <t>NCT U</t>
+  </si>
+  <si>
+    <t>NCT DREAM</t>
+  </si>
+  <si>
+    <t>NCT DOJAEJUNG</t>
+  </si>
+  <si>
+    <t>MINHO</t>
+  </si>
+  <si>
+    <t>MAX CHANGMIN</t>
+  </si>
+  <si>
+    <t>MARK</t>
+  </si>
+  <si>
+    <t>LUCAS</t>
+  </si>
+  <si>
+    <t>LEETEUK</t>
+  </si>
+  <si>
+    <t>LEE JAERYOUNG</t>
+  </si>
+  <si>
+    <t>LEE DONGWOO</t>
+  </si>
+  <si>
+    <t>LEE CHEOLWOO</t>
+  </si>
+  <si>
+    <t>LAMI</t>
+  </si>
+  <si>
+    <t>KUN</t>
+  </si>
+  <si>
+    <t>KIM KYUNGSHIK</t>
+  </si>
+  <si>
+    <t>KIM JIWOO</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>KARINA</t>
+  </si>
+  <si>
+    <t>KANGTA</t>
+  </si>
+  <si>
+    <t>KANGIN</t>
+  </si>
+  <si>
+    <t>KAI</t>
+  </si>
+  <si>
+    <t>JUNGWOO</t>
+  </si>
+  <si>
+    <t>JOY</t>
+  </si>
+  <si>
+    <t>JONGHYUN</t>
+  </si>
+  <si>
+    <t>JOHNNY</t>
+  </si>
+  <si>
+    <t>JISUNG</t>
+  </si>
+  <si>
+    <t>JENO</t>
+  </si>
+  <si>
+    <t>JAEMIN</t>
+  </si>
+  <si>
+    <t>JAEHYUN</t>
+  </si>
+  <si>
+    <t>JAEHEE</t>
+  </si>
+  <si>
+    <t>J-Min</t>
+  </si>
+  <si>
+    <t>IRENE</t>
+  </si>
+  <si>
+    <t>IMLAY</t>
+  </si>
+  <si>
+    <t>HYOYEON</t>
+  </si>
+  <si>
+    <t>HENDERY</t>
+  </si>
+  <si>
+    <t>HEECHUL</t>
+  </si>
+  <si>
+    <t>HAECHAN</t>
+  </si>
+  <si>
+    <t>GOT the beat</t>
+  </si>
+  <si>
+    <t>GISELLE</t>
+  </si>
+  <si>
+    <t>Girls’ Generation-TTS</t>
+  </si>
+  <si>
+    <t>GIRLS’ GENERATION-Oh!GG</t>
+  </si>
+  <si>
+    <t>GIRLS’ GENERATION</t>
+  </si>
+  <si>
+    <t>GINJO</t>
+  </si>
+  <si>
+    <t>EXO-SC</t>
+  </si>
+  <si>
+    <t>EXO-CBX</t>
+  </si>
+  <si>
+    <t>EUNSEOK</t>
+  </si>
+  <si>
+    <t>DOYOUNG</t>
+  </si>
+  <si>
+    <t>CHOI JONGYUN</t>
+  </si>
+  <si>
+    <t>CHO JUNYOUNG</t>
+  </si>
+  <si>
+    <t>CHENLE</t>
+  </si>
+  <si>
+    <t>CHEN</t>
+  </si>
+  <si>
+    <t>CHANYEOL</t>
+  </si>
+  <si>
+    <t>BoA</t>
+  </si>
+  <si>
+    <t>BAEKHYUN</t>
+  </si>
+  <si>
+    <t>ANTON</t>
   </si>
 </sst>
 </file>
@@ -319,7 +634,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -660,15 +1015,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0FEE81-6D47-3344-861D-2B54DE3A388F}">
-  <dimension ref="A1:A76"/>
+  <dimension ref="A1:A181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A1:A1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -693,373 +1048,902 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>33</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>43</v>
+        <v>153</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>55</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>46</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>2</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>16</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
         <v>60</v>
       </c>
     </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1 A128:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="A191:A1048576 A1">
+    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B1048576 A2:A57 B1">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="A191:A1048576 A1:A75">
+    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A77 A128:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A1:A75 A191:A1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A56">
+    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed artists not found on spotify from artist list
</commit_message>
<xml_diff>
--- a/data/artist_list.xlsx
+++ b/data/artist_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylergleeson/Documents/GitHub/kpop_analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7270C7ED-F7E2-0E49-9435-C87DB2EC847B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9883792-1CA3-E342-B519-73032EE878B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$174</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>EXO</t>
   </si>
@@ -278,15 +278,9 @@
     <t>YURI</t>
   </si>
   <si>
-    <t>YOU HOJEONG</t>
-  </si>
-  <si>
     <t>YOONA</t>
   </si>
   <si>
-    <t>YOON DAHOON</t>
-  </si>
-  <si>
     <t>YESUNG</t>
   </si>
   <si>
@@ -371,9 +365,6 @@
     <t>SOHEE</t>
   </si>
   <si>
-    <t>SM The Ballad</t>
-  </si>
-  <si>
     <t>SIWON</t>
   </si>
   <si>
@@ -446,12 +437,6 @@
     <t>LEETEUK</t>
   </si>
   <si>
-    <t>LEE JAERYOUNG</t>
-  </si>
-  <si>
-    <t>LEE DONGWOO</t>
-  </si>
-  <si>
     <t>LEE CHEOLWOO</t>
   </si>
   <si>
@@ -461,9 +446,6 @@
     <t>KUN</t>
   </si>
   <si>
-    <t>KIM KYUNGSHIK</t>
-  </si>
-  <si>
     <t>KIM JIWOO</t>
   </si>
   <si>
@@ -558,9 +540,6 @@
   </si>
   <si>
     <t>DOYOUNG</t>
-  </si>
-  <si>
-    <t>CHOI JONGYUN</t>
   </si>
   <si>
     <t>CHO JUNYOUNG</t>
@@ -995,9 +974,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0FEE81-6D47-3344-861D-2B54DE3A388F}">
-  <dimension ref="A1:A181"/>
+  <dimension ref="A1:A174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1026,7 +1007,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
@@ -1051,7 +1032,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
@@ -1066,7 +1047,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -1091,17 +1072,17 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
@@ -1111,817 +1092,782 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>171</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>0</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>164</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>163</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>159</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>143</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>67</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>139</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>137</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>136</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>134</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>72</v>
+        <v>129</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>131</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>130</v>
+        <v>41</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>126</v>
+        <v>33</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>123</v>
+        <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>96</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A75 A191:A1048576">
+  <conditionalFormatting sqref="A184:A1048576 A1:A74">
     <cfRule type="duplicateValues" dxfId="4" priority="1"/>
     <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A56">
-    <cfRule type="duplicateValues" dxfId="2" priority="16"/>
+  <conditionalFormatting sqref="A184:A1048576 A1">
+    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A191:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="1" priority="8"/>
+  <conditionalFormatting sqref="A184:A1048576 A1:A74">
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A191:A1048576 A1:A75">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  <conditionalFormatting sqref="A2:A55">
+    <cfRule type="duplicateValues" dxfId="0" priority="21"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
kpop artist list FIXED
</commit_message>
<xml_diff>
--- a/data/artist_list.xlsx
+++ b/data/artist_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylergleeson/Documents/GitHub/kpop_analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B623F5-2E44-4D46-844E-9A79B69C14BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC80FF44-ABDF-A54D-B0AE-7BD5B04D89DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>Artist</t>
   </si>
@@ -65,24 +65,12 @@
     <t>ZHOUMI</t>
   </si>
   <si>
-    <t>ZEROBASEONE</t>
-  </si>
-  <si>
-    <t>Zach Bryan</t>
-  </si>
-  <si>
-    <t>Yutaka Yamada</t>
-  </si>
-  <si>
     <t>YUTA</t>
   </si>
   <si>
     <t>YUSHI</t>
   </si>
   <si>
-    <t>Yuridia</t>
-  </si>
-  <si>
     <t>YURI</t>
   </si>
   <si>
@@ -92,24 +80,12 @@
     <t>Yoon Mirae</t>
   </si>
   <si>
-    <t>Yoko Shimomura</t>
-  </si>
-  <si>
-    <t>Yim Siwan</t>
-  </si>
-  <si>
     <t>YESUNG</t>
   </si>
   <si>
-    <t>Yeri Mua</t>
-  </si>
-  <si>
     <t>YERI</t>
   </si>
   <si>
-    <t>Yeeun</t>
-  </si>
-  <si>
     <t>YANGYANG</t>
   </si>
   <si>
@@ -122,18 +98,9 @@
     <t>WONBIN</t>
   </si>
   <si>
-    <t>Wolfgang Amadeus Mozart</t>
-  </si>
-  <si>
     <t>WJSN</t>
   </si>
   <si>
-    <t>witchxr</t>
-  </si>
-  <si>
-    <t>WiTCHX</t>
-  </si>
-  <si>
     <t>WinWin 楊安妮</t>
   </si>
   <si>
@@ -158,33 +125,12 @@
     <t>WayV</t>
   </si>
   <si>
-    <t>Victor Rivera Y Su Nuevo Estilo</t>
-  </si>
-  <si>
-    <t>VCHA</t>
-  </si>
-  <si>
-    <t>Vance Joy</t>
-  </si>
-  <si>
-    <t>Uzielito Mix</t>
-  </si>
-  <si>
-    <t>UV</t>
-  </si>
-  <si>
     <t>U-Know</t>
   </si>
   <si>
-    <t>TXTEK</t>
-  </si>
-  <si>
     <t>TXT</t>
   </si>
   <si>
-    <t>TWS</t>
-  </si>
-  <si>
     <t>TWICE</t>
   </si>
   <si>
@@ -194,33 +140,15 @@
     <t>TVXQ</t>
   </si>
   <si>
-    <t>Troye Sivan</t>
-  </si>
-  <si>
     <t>Treasure</t>
   </si>
   <si>
-    <t>TopGunn</t>
-  </si>
-  <si>
-    <t>TK &amp; The Holy Know-Nothings</t>
-  </si>
-  <si>
-    <t>TheFatRat</t>
-  </si>
-  <si>
-    <t>The Highwaymen</t>
-  </si>
-  <si>
     <t>The Boyz</t>
   </si>
   <si>
     <t>TEN</t>
   </si>
   <si>
-    <t>Taylor Swift</t>
-  </si>
-  <si>
     <t>TAEYONG</t>
   </si>
   <si>
@@ -233,15 +161,9 @@
     <t>TAEIL</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
     <t>Suzy</t>
   </si>
   <si>
-    <t>Supermode</t>
-  </si>
-  <si>
     <t>SuperM</t>
   </si>
   <si>
@@ -284,9 +206,6 @@
     <t>SOHEE</t>
   </si>
   <si>
-    <t>Skrapy</t>
-  </si>
-  <si>
     <t>SIWON</t>
   </si>
   <si>
@@ -296,18 +215,9 @@
     <t>SISTAR</t>
   </si>
   <si>
-    <t>Siona Swin</t>
-  </si>
-  <si>
     <t>SION</t>
   </si>
   <si>
-    <t>Silk City</t>
-  </si>
-  <si>
-    <t>Shotaro Shima</t>
-  </si>
-  <si>
     <t>SHOTARO</t>
   </si>
   <si>
@@ -329,45 +239,27 @@
     <t>SEULGI</t>
   </si>
   <si>
-    <t>Sergei Rachmaninoff</t>
-  </si>
-  <si>
     <t>SEHUN</t>
   </si>
   <si>
     <t>SAKUYA</t>
   </si>
   <si>
-    <t>Ryokuoushoku Shakai</t>
-  </si>
-  <si>
     <t>RYO</t>
   </si>
   <si>
     <t>RYEOWOOK</t>
   </si>
   <si>
-    <t>Ryan Gosling</t>
-  </si>
-  <si>
     <t>Rocket Punch</t>
   </si>
   <si>
-    <t>Riku Diamond</t>
-  </si>
-  <si>
     <t>RIKU</t>
   </si>
   <si>
     <t>RIIZE</t>
   </si>
   <si>
-    <t>Ricky Martin</t>
-  </si>
-  <si>
-    <t>Richy Mitch &amp; The Coal Miners</t>
-  </si>
-  <si>
     <t>RENJUN</t>
   </si>
   <si>
@@ -377,27 +269,15 @@
     <t>Red Velvet</t>
   </si>
   <si>
-    <t>reality.</t>
-  </si>
-  <si>
-    <t>Rauw Alejandro</t>
-  </si>
-  <si>
     <t>Raiden</t>
   </si>
   <si>
     <t>PURPLE KISS</t>
   </si>
   <si>
-    <t>Purple Disco Machine</t>
-  </si>
-  <si>
     <t>Pentagon</t>
   </si>
   <si>
-    <t>Ozuna</t>
-  </si>
-  <si>
     <t>ONEWE</t>
   </si>
   <si>
@@ -410,18 +290,12 @@
     <t>NU'EST</t>
   </si>
   <si>
-    <t>Noel Gallagher's High Flying Birds</t>
-  </si>
-  <si>
     <t>NINGNING</t>
   </si>
   <si>
     <t>NewJeans</t>
   </si>
   <si>
-    <t>Nestor En Bloque</t>
-  </si>
-  <si>
     <t>NCT WISH</t>
   </si>
   <si>
@@ -449,51 +323,21 @@
     <t>MOMOLAND</t>
   </si>
   <si>
-    <t>Mitchell Tenpenny</t>
-  </si>
-  <si>
-    <t>Miss fugu</t>
-  </si>
-  <si>
     <t>MIRAE</t>
   </si>
   <si>
     <t>MINHO</t>
   </si>
   <si>
-    <t>Mina</t>
-  </si>
-  <si>
-    <t>Miley Cyrus</t>
-  </si>
-  <si>
-    <t>miguel romano</t>
-  </si>
-  <si>
     <t>MAX CHANGMIN</t>
   </si>
   <si>
-    <t>Mark Ronson</t>
-  </si>
-  <si>
     <t>MARK</t>
   </si>
   <si>
-    <t>Maria Becerra</t>
-  </si>
-  <si>
-    <t>Marco Antonio Solís</t>
-  </si>
-  <si>
-    <t>Manuel Rodriguez</t>
-  </si>
-  <si>
     <t>MAMAMOO</t>
   </si>
   <si>
-    <t>Ludwig van Beethoven</t>
-  </si>
-  <si>
     <t>LUCAS</t>
   </si>
   <si>
@@ -503,7 +347,286 @@
     <t>LOONA</t>
   </si>
   <si>
-    <t>Lil Jon &amp; The East Side Boyz</t>
+    <t>(G)I-DLE</t>
+  </si>
+  <si>
+    <t>2PM</t>
+  </si>
+  <si>
+    <t>aespa</t>
+  </si>
+  <si>
+    <t>AILEE</t>
+  </si>
+  <si>
+    <t>ANTON</t>
+  </si>
+  <si>
+    <t>AOA</t>
+  </si>
+  <si>
+    <t>APRIL</t>
+  </si>
+  <si>
+    <t>ASTRO</t>
+  </si>
+  <si>
+    <t>ATEEZ</t>
+  </si>
+  <si>
+    <t>BAEKHYUN</t>
+  </si>
+  <si>
+    <t>BIGBANG</t>
+  </si>
+  <si>
+    <t>BLACKPINK</t>
+  </si>
+  <si>
+    <t>BoA</t>
+  </si>
+  <si>
+    <t>BOYFRIEND</t>
+  </si>
+  <si>
+    <t>BTOB</t>
+  </si>
+  <si>
+    <t>BTS</t>
+  </si>
+  <si>
+    <t>CHANYEOL</t>
+  </si>
+  <si>
+    <t>CHEN</t>
+  </si>
+  <si>
+    <t>CHENLE</t>
+  </si>
+  <si>
+    <t>Cherry Bullet</t>
+  </si>
+  <si>
+    <t>CHO JUNYOUNG</t>
+  </si>
+  <si>
+    <t>CHOI JONGYUN</t>
+  </si>
+  <si>
+    <t>CHOI SIWON</t>
+  </si>
+  <si>
+    <t>Chungha</t>
+  </si>
+  <si>
+    <t>CLC</t>
+  </si>
+  <si>
+    <t>CNBLUE</t>
+  </si>
+  <si>
+    <t>CRAVITY</t>
+  </si>
+  <si>
+    <t>DOYOUNG</t>
+  </si>
+  <si>
+    <t>ENHYPEN</t>
+  </si>
+  <si>
+    <t>EUNHYUK</t>
+  </si>
+  <si>
+    <t>EUNSEOK</t>
+  </si>
+  <si>
+    <t>EVERGLOW</t>
+  </si>
+  <si>
+    <t>EXO</t>
+  </si>
+  <si>
+    <t>EXO-CBX</t>
+  </si>
+  <si>
+    <t>EXO-SC</t>
+  </si>
+  <si>
+    <t>fromis_9</t>
+  </si>
+  <si>
+    <t>FTISLAND</t>
+  </si>
+  <si>
+    <t>GFRIEND</t>
+  </si>
+  <si>
+    <t>GINJO</t>
+  </si>
+  <si>
+    <t>Girls' Generation</t>
+  </si>
+  <si>
+    <t>GIRLS’ GENERATION</t>
+  </si>
+  <si>
+    <t>Girls' Generation-Oh!GG</t>
+  </si>
+  <si>
+    <t>GIRLS’ GENERATION-Oh!GG</t>
+  </si>
+  <si>
+    <t>Girls' Generation-TTS</t>
+  </si>
+  <si>
+    <t>Girls’ Generation-TTS</t>
+  </si>
+  <si>
+    <t>GISELLE</t>
+  </si>
+  <si>
+    <t>GOT the beat</t>
+  </si>
+  <si>
+    <t>GOT7</t>
+  </si>
+  <si>
+    <t>HAECHAN</t>
+  </si>
+  <si>
+    <t>HEECHUL</t>
+  </si>
+  <si>
+    <t>HENDERY</t>
+  </si>
+  <si>
+    <t>HYO</t>
+  </si>
+  <si>
+    <t>HYOYEON</t>
+  </si>
+  <si>
+    <t>iKON</t>
+  </si>
+  <si>
+    <t>INFINITE</t>
+  </si>
+  <si>
+    <t>IRENE</t>
+  </si>
+  <si>
+    <t>ITZY</t>
+  </si>
+  <si>
+    <t>IVE</t>
+  </si>
+  <si>
+    <t>IZ*ONE</t>
+  </si>
+  <si>
+    <t>JAEHEE</t>
+  </si>
+  <si>
+    <t>JAEHYUN</t>
+  </si>
+  <si>
+    <t>JAEMIN</t>
+  </si>
+  <si>
+    <t>Jay Park</t>
+  </si>
+  <si>
+    <t>JENO</t>
+  </si>
+  <si>
+    <t>JEON SOYEON</t>
+  </si>
+  <si>
+    <t>JISUNG</t>
+  </si>
+  <si>
+    <t>JOHNNY</t>
+  </si>
+  <si>
+    <t>JONGHYUN</t>
+  </si>
+  <si>
+    <t>JOY</t>
+  </si>
+  <si>
+    <t>JUNGWOO</t>
+  </si>
+  <si>
+    <t>K/DA</t>
+  </si>
+  <si>
+    <t>KAI</t>
+  </si>
+  <si>
+    <t>KANGIN</t>
+  </si>
+  <si>
+    <t>KANGTA</t>
+  </si>
+  <si>
+    <t>KARA</t>
+  </si>
+  <si>
+    <t>KARD</t>
+  </si>
+  <si>
+    <t>KARINA</t>
+  </si>
+  <si>
+    <t>Kep1er</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>KIM HEECHUL</t>
+  </si>
+  <si>
+    <t>KIM JIWOO</t>
+  </si>
+  <si>
+    <t>KIM KYUNGSHIK</t>
+  </si>
+  <si>
+    <t>KUN</t>
+  </si>
+  <si>
+    <t>KYUHYUN</t>
+  </si>
+  <si>
+    <t>LAMI</t>
+  </si>
+  <si>
+    <t>Le Sserafim</t>
+  </si>
+  <si>
+    <t>LEE CHEOLWOO</t>
+  </si>
+  <si>
+    <t>LEE DONGWOO</t>
+  </si>
+  <si>
+    <t>LEE JAERYOUNG</t>
+  </si>
+  <si>
+    <t>LEETEUK</t>
+  </si>
+  <si>
+    <t>Red Velvet – IRENE &amp; SEULGI</t>
+  </si>
+  <si>
+    <t>SM The Ballad</t>
+  </si>
+  <si>
+    <t>YOON DAHOON</t>
+  </si>
+  <si>
+    <t>YOU HOJEONG</t>
   </si>
 </sst>
 </file>
@@ -947,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0FEE81-6D47-3344-861D-2B54DE3A388F}">
-  <dimension ref="A1:A157"/>
+  <dimension ref="A1:A196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A2" sqref="A2:A196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -965,800 +1088,991 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>100</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>91</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>168</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>177</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>77</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>75</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>73</v>
+        <v>182</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>72</v>
+        <v>183</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>70</v>
+        <v>185</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>69</v>
+        <v>186</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>68</v>
+        <v>187</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>66</v>
+        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>65</v>
+        <v>190</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>64</v>
+        <v>191</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>33</v>
+        <v>192</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>193</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>1</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A488:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="7" priority="12"/>
+  <conditionalFormatting sqref="A25:A151">
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A488:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25:A151">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25:A151">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed unclassified artists from artist list with uri errors
</commit_message>
<xml_diff>
--- a/data/artist_list.xlsx
+++ b/data/artist_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylergleeson/Documents/GitHub/kpop_analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC80FF44-ABDF-A54D-B0AE-7BD5B04D89DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0437E5A0-F1FF-E94B-8B20-F6FC8D8D9A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>Artist</t>
   </si>
@@ -410,9 +410,6 @@
     <t>CHO JUNYOUNG</t>
   </si>
   <si>
-    <t>CHOI JONGYUN</t>
-  </si>
-  <si>
     <t>CHOI SIWON</t>
   </si>
   <si>
@@ -590,9 +587,6 @@
     <t>KIM JIWOO</t>
   </si>
   <si>
-    <t>KIM KYUNGSHIK</t>
-  </si>
-  <si>
     <t>KUN</t>
   </si>
   <si>
@@ -608,9 +602,6 @@
     <t>LEE CHEOLWOO</t>
   </si>
   <si>
-    <t>LEE DONGWOO</t>
-  </si>
-  <si>
     <t>LEE JAERYOUNG</t>
   </si>
   <si>
@@ -618,15 +609,6 @@
   </si>
   <si>
     <t>Red Velvet – IRENE &amp; SEULGI</t>
-  </si>
-  <si>
-    <t>SM The Ballad</t>
-  </si>
-  <si>
-    <t>YOON DAHOON</t>
-  </si>
-  <si>
-    <t>YOU HOJEONG</t>
   </si>
 </sst>
 </file>
@@ -1070,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0FEE81-6D47-3344-861D-2B54DE3A388F}">
-  <dimension ref="A1:A196"/>
+  <dimension ref="A1:A190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A196"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="A186" sqref="A186:XFD186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1218,12 +1200,12 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
@@ -1358,12 +1340,12 @@
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>155</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>2</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
@@ -1388,12 +1370,12 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>160</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
@@ -1538,541 +1520,511 @@
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>189</v>
+        <v>101</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>190</v>
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>191</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>76</v>
+        <v>189</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>192</v>
+        <v>71</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>193</v>
+        <v>51</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A191" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A193" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A194" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A25:A151">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  <conditionalFormatting sqref="A482:A1048576 A1">
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A488:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
+  <conditionalFormatting sqref="A24:A147">
+    <cfRule type="duplicateValues" dxfId="3" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="32"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
one additional undefined artist uri removed
</commit_message>
<xml_diff>
--- a/data/artist_list.xlsx
+++ b/data/artist_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylergleeson/Documents/GitHub/kpop_analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0437E5A0-F1FF-E94B-8B20-F6FC8D8D9A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5E9DFF-A947-AF42-8C35-8F6A8F183E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t>Artist</t>
   </si>
@@ -600,9 +600,6 @@
   </si>
   <si>
     <t>LEE CHEOLWOO</t>
-  </si>
-  <si>
-    <t>LEE JAERYOUNG</t>
   </si>
   <si>
     <t>LEETEUK</t>
@@ -1052,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0FEE81-6D47-3344-861D-2B54DE3A388F}">
-  <dimension ref="A1:A190"/>
+  <dimension ref="A1:A189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="A186" sqref="A186:XFD186"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90:XFD90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1515,516 +1512,511 @@
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>188</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>74</v>
+        <v>188</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>189</v>
+        <v>73</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A190" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A482:A1048576 A1">
+  <conditionalFormatting sqref="A481:A1048576 A1">
     <cfRule type="duplicateValues" dxfId="7" priority="5"/>
     <cfRule type="duplicateValues" dxfId="6" priority="9"/>
     <cfRule type="duplicateValues" dxfId="5" priority="10"/>
     <cfRule type="duplicateValues" dxfId="4" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A24:A147">
-    <cfRule type="duplicateValues" dxfId="3" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="31"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="32"/>
+  <conditionalFormatting sqref="A24:A146">
+    <cfRule type="duplicateValues" dxfId="3" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="36"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upload filtered kpop data file correct
</commit_message>
<xml_diff>
--- a/data/artist_list.xlsx
+++ b/data/artist_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylergleeson/Documents/GitHub/kpop_analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5E9DFF-A947-AF42-8C35-8F6A8F183E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755AD1F3-09FA-B442-9AEF-CE63E3A5B025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -753,9 +753,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -793,7 +793,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -899,7 +899,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1041,7 +1041,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0FEE81-6D47-3344-861D-2B54DE3A388F}">
   <dimension ref="A1:A189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90:XFD90"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2006,17 +2006,17 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A24:A146">
+    <cfRule type="duplicateValues" dxfId="7" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="36"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A481:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24:A146">
-    <cfRule type="duplicateValues" dxfId="3" priority="33"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="35"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
final kpop data set
</commit_message>
<xml_diff>
--- a/data/artist_list.xlsx
+++ b/data/artist_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylergleeson/Documents/GitHub/kpop_analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B703122-F395-7442-A75C-3F9A381711E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A82A4DA-510D-6941-9E44-75BD16F8FA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="20040" xr2:uid="{6EA75BC8-7E97-A641-A26D-A554D3532DC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -832,7 +832,7 @@
   <dimension ref="A1:A129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>